<commit_message>
fix: modified country names, host name logic
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/ReferenceSummary_Genbank_Feb25.xlsx
+++ b/Pubmed/CCHF/ReferenceSummary_Genbank_Feb25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/Library/CloudStorage/Dropbox/Shared/___SystematicReviewsAI/CCHF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Desktop/HIV/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE29215-EEB8-5D41-BE83-F4A986268F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E599AF8D-0C6C-6941-AC31-5346C5F0926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1600" windowWidth="34540" windowHeight="20000" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
+    <workbookView xWindow="20" yWindow="900" windowWidth="34540" windowHeight="20000" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$27</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1109,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4482E4AD-E7FE-EC42-9928-56B66BBA47E4}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1131,7 @@
     <col min="14" max="14" width="10.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="34.83203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="18.1640625" style="1" customWidth="1"/>
     <col min="19" max="20" width="10.83203125" style="1" customWidth="1"/>
     <col min="21" max="22" width="17.1640625" style="1" customWidth="1"/>

</xml_diff>